<commit_message>
check ist calidad p1335
</commit_message>
<xml_diff>
--- a/Proyectos/2015/11/P1335 - 2HR, Jorge Armando Hernández_OC/Calidad/Checklist_Calidad_151209.xlsx
+++ b/Proyectos/2015/11/P1335 - 2HR, Jorge Armando Hernández_OC/Calidad/Checklist_Calidad_151209.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" state="visible" r:id="rId2"/>
@@ -14622,7 +14622,7 @@
       </c>
       <c r="C15" s="17" t="n">
         <f aca="false">COUNTA(procesos!C11:C18)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" s="18" t="n">
         <f aca="false">COUNTIF(procesos!C11:C18,"x")/(COUNTIF((procesos!C11:C18),"x")+COUNTIF((procesos!D11:D18),"x"))</f>
@@ -21067,8 +21067,8 @@
   </sheetPr>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21167,7 +21167,7 @@
     </row>
     <row r="7" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="39" t="s">
         <v>13</v>
       </c>
@@ -21181,7 +21181,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="39"/>
       <c r="B10" s="39"/>
       <c r="C10" s="42" t="s">
@@ -21195,21 +21195,21 @@
       </c>
       <c r="F10" s="41"/>
     </row>
-    <row r="11" s="38" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="44" t="n">
         <v>1</v>
       </c>
       <c r="B11" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
       <c r="F11" s="45"/>
     </row>
-    <row r="12" s="38" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="44" t="n">
         <v>2</v>
       </c>
@@ -21223,7 +21223,7 @@
       <c r="E12" s="44"/>
       <c r="F12" s="45"/>
     </row>
-    <row r="13" s="38" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="44" t="n">
         <v>3</v>
       </c>
@@ -21237,7 +21237,7 @@
       <c r="E13" s="44"/>
       <c r="F13" s="45"/>
     </row>
-    <row r="14" s="38" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="44" t="n">
         <v>4</v>
       </c>
@@ -21251,7 +21251,7 @@
       <c r="E14" s="44"/>
       <c r="F14" s="45"/>
     </row>
-    <row r="15" s="38" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="44" t="n">
         <v>5</v>
       </c>
@@ -21265,7 +21265,7 @@
       <c r="E15" s="44"/>
       <c r="F15" s="45"/>
     </row>
-    <row r="16" s="38" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="44" t="n">
         <v>6</v>
       </c>
@@ -21279,7 +21279,7 @@
       <c r="E16" s="44"/>
       <c r="F16" s="45"/>
     </row>
-    <row r="17" s="38" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="44" t="n">
         <v>7</v>
       </c>
@@ -21293,7 +21293,7 @@
       <c r="E17" s="44"/>
       <c r="F17" s="45"/>
     </row>
-    <row r="18" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="44" t="n">
         <v>8</v>
       </c>
@@ -22722,7 +22722,7 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>